<commit_message>
Update b2b import lead demo file
</commit_message>
<xml_diff>
--- a/ui/buyer_catalogue/app/sample_files/b2b_import_lead.xlsx
+++ b/ui/buyer_catalogue/app/sample_files/b2b_import_lead.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t xml:space="preserve">Phone Number</t>
   </si>
@@ -55,6 +55,9 @@
     <t xml:space="preserve">Comment</t>
   </si>
   <si>
+    <t xml:space="preserve">Submitted</t>
+  </si>
+  <si>
     <t xml:space="preserve">Education</t>
   </si>
   <si>
@@ -76,6 +79,9 @@
     <t xml:space="preserve">Test</t>
   </si>
   <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
     <t xml:space="preserve">Real Estate</t>
   </si>
   <si>
@@ -94,13 +100,7 @@
     <t xml:space="preserve">Test2</t>
   </si>
   <si>
-    <t xml:space="preserve">juhu dhara complex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mumbai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Behala</t>
+    <t xml:space="preserve">Yes</t>
   </si>
 </sst>
 </file>
@@ -110,7 +110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -138,11 +138,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -196,7 +191,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -217,13 +212,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="20.74"/>
@@ -264,31 +259,37 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>9833179041</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -296,77 +297,54 @@
         <v>1215465447454</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="A4" s="0" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="K4" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="L4" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>123456</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding two extra columns for capturing the satisfaction level for existing partners
</commit_message>
<xml_diff>
--- a/ui/buyer_catalogue/app/sample_files/b2b_import_lead.xlsx
+++ b/ui/buyer_catalogue/app/sample_files/b2b_import_lead.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t xml:space="preserve">Phone Number</t>
   </si>
@@ -40,6 +40,12 @@
     <t xml:space="preserve">Current partner</t>
   </si>
   <si>
+    <t xml:space="preserve">Current Patner Feedback</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Patner Feedback Reason</t>
+  </si>
+  <si>
     <t xml:space="preserve">Prefered Partners</t>
   </si>
   <si>
@@ -64,6 +70,12 @@
     <t xml:space="preserve">Ecommerce service</t>
   </si>
   <si>
+    <t xml:space="preserve">Satisfied</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Anarock, Ecommerce service</t>
   </si>
   <si>
@@ -88,6 +100,12 @@
     <t xml:space="preserve">Anarock</t>
   </si>
   <si>
+    <t xml:space="preserve">Dissatisfied</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test 3</t>
+  </si>
+  <si>
     <t xml:space="preserve">next 2-4 months</t>
   </si>
   <si>
@@ -101,6 +119,9 @@
   </si>
   <si>
     <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extremely Dissatisfied</t>
   </si>
 </sst>
 </file>
@@ -212,17 +233,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="20.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="36.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="20.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.77"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -262,34 +286,46 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>9833179041</v>
+        <v>44444444441</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -297,25 +333,31 @@
         <v>1215465447454</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>26</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -323,28 +365,31 @@
         <v>123456</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed in b2b lead distribution
</commit_message>
<xml_diff>
--- a/ui/buyer_catalogue/app/sample_files/b2b_import_lead.xlsx
+++ b/ui/buyer_catalogue/app/sample_files/b2b_import_lead.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="supplier_upload" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">Phone Number</t>
   </si>
@@ -58,6 +58,12 @@
     <t xml:space="preserve">Meating Timeline</t>
   </si>
   <si>
+    <t xml:space="preserve">L1 Answers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L2 Answers</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lead Status</t>
   </si>
   <si>
@@ -73,15 +79,12 @@
     <t xml:space="preserve">School</t>
   </si>
   <si>
-    <t xml:space="preserve">ABC Org</t>
+    <t xml:space="preserve">Ecommerce service</t>
   </si>
   <si>
     <t xml:space="preserve">Satisfied</t>
   </si>
   <si>
-    <t xml:space="preserve">Test 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Anarock, Ecommerce service</t>
   </si>
   <si>
@@ -91,46 +94,19 @@
     <t xml:space="preserve">Immediate</t>
   </si>
   <si>
+    <t xml:space="preserve">ABC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC22</t>
+  </si>
+  <si>
     <t xml:space="preserve">Very Deep Lead</t>
   </si>
   <si>
     <t xml:space="preserve">Test</t>
   </si>
   <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Real Estate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Builders</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anarock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dissatisfied</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">next 2-4 months</t>
-  </si>
-  <si>
-    <t xml:space="preserve">after 2 months</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lead</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extremely Dissatisfied</t>
   </si>
 </sst>
 </file>
@@ -227,36 +203,40 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="36.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="30.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="24.73"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -305,119 +285,58 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>3333333333</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>15</v>
+        <v>9810062259</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="J2" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="K2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>1215465447454</v>
-      </c>
-      <c r="E3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="P2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="Q2" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>123456</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="N4" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="O4" s="0" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>